<commit_message>
removed some false positive entries
</commit_message>
<xml_diff>
--- a/add-in-ids/add-ins-using-exchange-tokens.xlsx
+++ b/add-in-ids/add-ins-using-exchange-tokens.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DD20CF-B37A-46F4-92D3-33ED68CC4748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E50CCF7-E62E-4438-B3F7-86827CD0CAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="37710" windowHeight="14130" xr2:uid="{8FF931F1-CAD9-4954-9038-88E82260DB46}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{8FF931F1-CAD9-4954-9038-88E82260DB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Add-ins list" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2759" uniqueCount="2648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2753" uniqueCount="2642">
   <si>
     <t>AssetID</t>
   </si>
@@ -936,15 +936,6 @@
     <t>Office2SharePoint</t>
   </si>
   <si>
-    <t>wa104380690</t>
-  </si>
-  <si>
-    <t>C83ECF7B-2C0F-49FC-942D-926C7EFF6B4D</t>
-  </si>
-  <si>
-    <t>Content Chooser</t>
-  </si>
-  <si>
     <t>wa104380691</t>
   </si>
   <si>
@@ -4813,15 +4804,6 @@
   </si>
   <si>
     <t>Signulu for Outlook</t>
-  </si>
-  <si>
-    <t>wa200003062</t>
-  </si>
-  <si>
-    <t>c5e867f6-e0a6-470f-9721-2d50ed3f02fd</t>
-  </si>
-  <si>
-    <t>Mail Signature</t>
   </si>
   <si>
     <t>wa200003064</t>
@@ -8059,8 +8041,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}" name="Table1" displayName="Table1" ref="A1:C921" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C921" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}" name="Table1" displayName="Table1" ref="A1:C919" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C919" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{39B649A1-0CDF-46AA-A276-6F4F89255D96}" name="AssetID"/>
     <tableColumn id="2" xr3:uid="{C79A1EFF-47FF-488B-A562-E9848648C952}" name="AppId"/>
@@ -8387,10 +8369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3293B4AA-89CE-4E6A-9112-DA5B905DDA88}">
-  <dimension ref="A1:C921"/>
+  <dimension ref="A1:C919"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8406,7 +8388,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2647</v>
+        <v>2641</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -9526,7 +9508,7 @@
       <c r="A104" t="s">
         <v>304</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="1" t="s">
         <v>305</v>
       </c>
       <c r="C104" t="s">
@@ -9537,7 +9519,7 @@
       <c r="A105" t="s">
         <v>307</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" t="s">
         <v>308</v>
       </c>
       <c r="C105" t="s">
@@ -10208,7 +10190,7 @@
       <c r="A166" t="s">
         <v>490</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="1" t="s">
         <v>491</v>
       </c>
       <c r="C166" t="s">
@@ -10219,7 +10201,7 @@
       <c r="A167" t="s">
         <v>493</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" t="s">
         <v>494</v>
       </c>
       <c r="C167" t="s">
@@ -10267,18 +10249,18 @@
         <v>506</v>
       </c>
       <c r="C171" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>507</v>
+      </c>
+      <c r="B172" t="s">
         <v>508</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>509</v>
-      </c>
-      <c r="C172" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -10913,18 +10895,18 @@
         <v>681</v>
       </c>
       <c r="B230" t="s">
+        <v>458</v>
+      </c>
+      <c r="C230" t="s">
         <v>682</v>
-      </c>
-      <c r="C230" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>683</v>
+      </c>
+      <c r="B231" t="s">
         <v>684</v>
-      </c>
-      <c r="B231" t="s">
-        <v>461</v>
       </c>
       <c r="C231" t="s">
         <v>685</v>
@@ -11518,15 +11500,15 @@
         <v>845</v>
       </c>
       <c r="B285" t="s">
-        <v>846</v>
+        <v>290</v>
       </c>
       <c r="C285" t="s">
-        <v>847</v>
+        <v>291</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B286" t="s">
         <v>290</v>
@@ -11537,7 +11519,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B287" t="s">
         <v>290</v>
@@ -11548,7 +11530,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B288" t="s">
         <v>290</v>
@@ -11559,7 +11541,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B289" t="s">
         <v>290</v>
@@ -11570,7 +11552,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B290" t="s">
         <v>290</v>
@@ -11581,13 +11563,13 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
+        <v>851</v>
+      </c>
+      <c r="B291" t="s">
+        <v>852</v>
+      </c>
+      <c r="C291" t="s">
         <v>853</v>
-      </c>
-      <c r="B291" t="s">
-        <v>290</v>
-      </c>
-      <c r="C291" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -11606,15 +11588,15 @@
         <v>857</v>
       </c>
       <c r="B293" t="s">
-        <v>858</v>
+        <v>290</v>
       </c>
       <c r="C293" t="s">
-        <v>859</v>
+        <v>291</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B294" t="s">
         <v>290</v>
@@ -11625,7 +11607,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B295" t="s">
         <v>290</v>
@@ -11636,7 +11618,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B296" t="s">
         <v>290</v>
@@ -11647,13 +11629,13 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
+        <v>861</v>
+      </c>
+      <c r="B297" t="s">
+        <v>862</v>
+      </c>
+      <c r="C297" t="s">
         <v>863</v>
-      </c>
-      <c r="B297" t="s">
-        <v>290</v>
-      </c>
-      <c r="C297" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -11672,21 +11654,21 @@
         <v>867</v>
       </c>
       <c r="B299" t="s">
-        <v>868</v>
+        <v>290</v>
       </c>
       <c r="C299" t="s">
-        <v>869</v>
+        <v>291</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
+        <v>868</v>
+      </c>
+      <c r="B300" t="s">
+        <v>869</v>
+      </c>
+      <c r="C300" t="s">
         <v>870</v>
-      </c>
-      <c r="B300" t="s">
-        <v>290</v>
-      </c>
-      <c r="C300" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -11694,15 +11676,15 @@
         <v>871</v>
       </c>
       <c r="B301" t="s">
-        <v>872</v>
+        <v>290</v>
       </c>
       <c r="C301" t="s">
-        <v>873</v>
+        <v>291</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B302" t="s">
         <v>290</v>
@@ -11713,13 +11695,13 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
+        <v>873</v>
+      </c>
+      <c r="B303" t="s">
+        <v>874</v>
+      </c>
+      <c r="C303" t="s">
         <v>875</v>
-      </c>
-      <c r="B303" t="s">
-        <v>290</v>
-      </c>
-      <c r="C303" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -11782,21 +11764,21 @@
         <v>891</v>
       </c>
       <c r="B309" t="s">
-        <v>892</v>
+        <v>290</v>
       </c>
       <c r="C309" t="s">
-        <v>893</v>
+        <v>291</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
+        <v>892</v>
+      </c>
+      <c r="B310" t="s">
+        <v>893</v>
+      </c>
+      <c r="C310" t="s">
         <v>894</v>
-      </c>
-      <c r="B310" t="s">
-        <v>290</v>
-      </c>
-      <c r="C310" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -11804,15 +11786,15 @@
         <v>895</v>
       </c>
       <c r="B311" t="s">
-        <v>896</v>
+        <v>290</v>
       </c>
       <c r="C311" t="s">
-        <v>897</v>
+        <v>291</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B312" t="s">
         <v>290</v>
@@ -11823,7 +11805,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B313" t="s">
         <v>290</v>
@@ -11834,7 +11816,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B314" t="s">
         <v>290</v>
@@ -11845,7 +11827,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="B315" t="s">
         <v>290</v>
@@ -11856,7 +11838,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B316" t="s">
         <v>290</v>
@@ -11867,7 +11849,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B317" t="s">
         <v>290</v>
@@ -11878,7 +11860,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B318" t="s">
         <v>290</v>
@@ -11889,7 +11871,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B319" t="s">
         <v>290</v>
@@ -11900,7 +11882,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B320" t="s">
         <v>290</v>
@@ -11911,7 +11893,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B321" t="s">
         <v>290</v>
@@ -11922,7 +11904,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B322" t="s">
         <v>290</v>
@@ -11933,7 +11915,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B323" t="s">
         <v>290</v>
@@ -11944,7 +11926,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B324" t="s">
         <v>290</v>
@@ -11955,7 +11937,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B325" t="s">
         <v>290</v>
@@ -11966,7 +11948,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B326" t="s">
         <v>290</v>
@@ -11977,7 +11959,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B327" t="s">
         <v>290</v>
@@ -11988,7 +11970,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B328" t="s">
         <v>290</v>
@@ -11999,7 +11981,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="B329" t="s">
         <v>290</v>
@@ -12010,7 +11992,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B330" t="s">
         <v>290</v>
@@ -12021,7 +12003,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="B331" t="s">
         <v>290</v>
@@ -12032,7 +12014,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B332" t="s">
         <v>290</v>
@@ -12043,13 +12025,13 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
+        <v>917</v>
+      </c>
+      <c r="B333" t="s">
+        <v>918</v>
+      </c>
+      <c r="C333" t="s">
         <v>919</v>
-      </c>
-      <c r="B333" t="s">
-        <v>290</v>
-      </c>
-      <c r="C333" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
@@ -12057,15 +12039,15 @@
         <v>920</v>
       </c>
       <c r="B334" t="s">
-        <v>921</v>
+        <v>290</v>
       </c>
       <c r="C334" t="s">
-        <v>922</v>
+        <v>291</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B335" t="s">
         <v>290</v>
@@ -12076,7 +12058,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B336" t="s">
         <v>290</v>
@@ -12087,7 +12069,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B337" t="s">
         <v>290</v>
@@ -12098,7 +12080,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="B338" t="s">
         <v>290</v>
@@ -12109,13 +12091,13 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
+        <v>925</v>
+      </c>
+      <c r="B339" t="s">
+        <v>926</v>
+      </c>
+      <c r="C339" t="s">
         <v>927</v>
-      </c>
-      <c r="B339" t="s">
-        <v>290</v>
-      </c>
-      <c r="C339" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -12123,15 +12105,15 @@
         <v>928</v>
       </c>
       <c r="B340" t="s">
-        <v>929</v>
+        <v>290</v>
       </c>
       <c r="C340" t="s">
-        <v>930</v>
+        <v>291</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B341" t="s">
         <v>290</v>
@@ -12142,13 +12124,13 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
+        <v>930</v>
+      </c>
+      <c r="B342" t="s">
+        <v>931</v>
+      </c>
+      <c r="C342" t="s">
         <v>932</v>
-      </c>
-      <c r="B342" t="s">
-        <v>290</v>
-      </c>
-      <c r="C342" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -12181,18 +12163,18 @@
         <v>940</v>
       </c>
       <c r="C345" t="s">
-        <v>941</v>
+        <v>291</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
+        <v>941</v>
+      </c>
+      <c r="B346" t="s">
         <v>942</v>
       </c>
-      <c r="B346" t="s">
+      <c r="C346" t="s">
         <v>943</v>
-      </c>
-      <c r="C346" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -12412,18 +12394,18 @@
         <v>1002</v>
       </c>
       <c r="C366" t="s">
-        <v>1003</v>
+        <v>291</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B367" t="s">
         <v>1004</v>
       </c>
-      <c r="B367" t="s">
+      <c r="C367" t="s">
         <v>1005</v>
-      </c>
-      <c r="C367" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -12431,21 +12413,21 @@
         <v>1006</v>
       </c>
       <c r="B368" t="s">
-        <v>1007</v>
+        <v>38</v>
       </c>
       <c r="C368" t="s">
-        <v>1008</v>
+        <v>39</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B369" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C369" t="s">
         <v>1009</v>
-      </c>
-      <c r="B369" t="s">
-        <v>38</v>
-      </c>
-      <c r="C369" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -12453,21 +12435,21 @@
         <v>1010</v>
       </c>
       <c r="B370" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="C370" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B371" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C371" t="s">
         <v>1013</v>
-      </c>
-      <c r="B371" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C371" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -12761,29 +12743,29 @@
         <v>1092</v>
       </c>
       <c r="B398" t="s">
-        <v>1093</v>
+        <v>1002</v>
       </c>
       <c r="C398" t="s">
-        <v>1094</v>
+        <v>291</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B399" t="s">
-        <v>1005</v>
+        <v>206</v>
       </c>
       <c r="C399" t="s">
-        <v>291</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B400" t="s">
         <v>1096</v>
-      </c>
-      <c r="B400" t="s">
-        <v>206</v>
       </c>
       <c r="C400" t="s">
         <v>1097</v>
@@ -13003,18 +12985,18 @@
         <v>1155</v>
       </c>
       <c r="B420" t="s">
+        <v>646</v>
+      </c>
+      <c r="C420" t="s">
         <v>1156</v>
-      </c>
-      <c r="C420" t="s">
-        <v>1157</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B421" t="s">
         <v>1158</v>
-      </c>
-      <c r="B421" t="s">
-        <v>649</v>
       </c>
       <c r="C421" t="s">
         <v>1159</v>
@@ -13101,7 +13083,7 @@
       <c r="A429" t="s">
         <v>1181</v>
       </c>
-      <c r="B429" t="s">
+      <c r="B429" s="1" t="s">
         <v>1182</v>
       </c>
       <c r="C429" t="s">
@@ -13112,7 +13094,7 @@
       <c r="A430" t="s">
         <v>1184</v>
       </c>
-      <c r="B430" s="1" t="s">
+      <c r="B430" t="s">
         <v>1185</v>
       </c>
       <c r="C430" t="s">
@@ -13233,7 +13215,7 @@
       <c r="A441" t="s">
         <v>1217</v>
       </c>
-      <c r="B441" t="s">
+      <c r="B441" s="1" t="s">
         <v>1218</v>
       </c>
       <c r="C441" t="s">
@@ -13244,7 +13226,7 @@
       <c r="A442" t="s">
         <v>1220</v>
       </c>
-      <c r="B442" s="1" t="s">
+      <c r="B442" t="s">
         <v>1221</v>
       </c>
       <c r="C442" t="s">
@@ -13321,7 +13303,7 @@
       <c r="A449" t="s">
         <v>1241</v>
       </c>
-      <c r="B449" t="s">
+      <c r="B449" s="1" t="s">
         <v>1242</v>
       </c>
       <c r="C449" t="s">
@@ -13332,7 +13314,7 @@
       <c r="A450" t="s">
         <v>1244</v>
       </c>
-      <c r="B450" s="1" t="s">
+      <c r="B450" t="s">
         <v>1245</v>
       </c>
       <c r="C450" t="s">
@@ -13541,7 +13523,7 @@
       <c r="A469" t="s">
         <v>1301</v>
       </c>
-      <c r="B469" t="s">
+      <c r="B469" s="1" t="s">
         <v>1302</v>
       </c>
       <c r="C469" t="s">
@@ -13552,7 +13534,7 @@
       <c r="A470" t="s">
         <v>1304</v>
       </c>
-      <c r="B470" s="1" t="s">
+      <c r="B470" t="s">
         <v>1305</v>
       </c>
       <c r="C470" t="s">
@@ -13684,7 +13666,7 @@
       <c r="A482" t="s">
         <v>1340</v>
       </c>
-      <c r="B482" t="s">
+      <c r="B482" s="1" t="s">
         <v>1341</v>
       </c>
       <c r="C482" t="s">
@@ -13695,7 +13677,7 @@
       <c r="A483" t="s">
         <v>1343</v>
       </c>
-      <c r="B483" s="1" t="s">
+      <c r="B483" t="s">
         <v>1344</v>
       </c>
       <c r="C483" t="s">
@@ -13773,21 +13755,21 @@
         <v>1364</v>
       </c>
       <c r="B490" t="s">
-        <v>1365</v>
+        <v>1002</v>
       </c>
       <c r="C490" t="s">
-        <v>1366</v>
+        <v>291</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B491" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C491" t="s">
         <v>1367</v>
-      </c>
-      <c r="B491" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C491" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.25">
@@ -14370,18 +14352,18 @@
         <v>1525</v>
       </c>
       <c r="C544" t="s">
-        <v>1526</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B545" t="s">
         <v>1527</v>
       </c>
-      <c r="B545" t="s">
+      <c r="C545" t="s">
         <v>1528</v>
-      </c>
-      <c r="C545" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.25">
@@ -14389,18 +14371,18 @@
         <v>1529</v>
       </c>
       <c r="B546" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C546" t="s">
         <v>1530</v>
-      </c>
-      <c r="C546" t="s">
-        <v>1531</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B547" t="s">
         <v>1532</v>
-      </c>
-      <c r="B547" t="s">
-        <v>1516</v>
       </c>
       <c r="C547" t="s">
         <v>1533</v>
@@ -14840,29 +14822,29 @@
         <v>1651</v>
       </c>
       <c r="B587" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C587" t="s">
         <v>1652</v>
-      </c>
-      <c r="C587" t="s">
-        <v>1653</v>
       </c>
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B588" t="s">
         <v>1654</v>
       </c>
-      <c r="B588" t="s">
+      <c r="C588" t="s">
         <v>1655</v>
-      </c>
-      <c r="C588" t="s">
-        <v>1656</v>
       </c>
     </row>
     <row r="589" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B589" t="s">
         <v>1657</v>
-      </c>
-      <c r="B589" t="s">
-        <v>1516</v>
       </c>
       <c r="C589" t="s">
         <v>1658</v>
@@ -15316,29 +15298,29 @@
         <v>1780</v>
       </c>
       <c r="C630" t="s">
-        <v>1781</v>
+        <v>626</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B631" t="s">
         <v>1782</v>
       </c>
-      <c r="B631" t="s">
+      <c r="C631" t="s">
         <v>1783</v>
-      </c>
-      <c r="C631" t="s">
-        <v>1784</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B632" t="s">
         <v>1785</v>
       </c>
-      <c r="B632" t="s">
+      <c r="C632" t="s">
         <v>1786</v>
-      </c>
-      <c r="C632" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.25">
@@ -15734,29 +15716,29 @@
         <v>1893</v>
       </c>
       <c r="C668" t="s">
-        <v>1894</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B669" t="s">
         <v>1895</v>
       </c>
-      <c r="B669" t="s">
+      <c r="C669" t="s">
         <v>1896</v>
-      </c>
-      <c r="C669" t="s">
-        <v>1897</v>
       </c>
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B670" t="s">
         <v>1898</v>
       </c>
-      <c r="B670" t="s">
+      <c r="C670" t="s">
         <v>1899</v>
-      </c>
-      <c r="C670" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="671" spans="1:3" x14ac:dyDescent="0.25">
@@ -15954,29 +15936,29 @@
         <v>1952</v>
       </c>
       <c r="C688" t="s">
-        <v>1953</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B689" t="s">
         <v>1954</v>
       </c>
-      <c r="B689" t="s">
+      <c r="C689" t="s">
         <v>1955</v>
-      </c>
-      <c r="C689" t="s">
-        <v>1956</v>
       </c>
     </row>
     <row r="690" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B690" t="s">
         <v>1957</v>
       </c>
-      <c r="B690" t="s">
+      <c r="C690" t="s">
         <v>1958</v>
-      </c>
-      <c r="C690" t="s">
-        <v>1409</v>
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
@@ -16746,29 +16728,29 @@
         <v>2167</v>
       </c>
       <c r="C760" t="s">
-        <v>2168</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B761" t="s">
         <v>2169</v>
       </c>
-      <c r="B761" t="s">
+      <c r="C761" t="s">
         <v>2170</v>
-      </c>
-      <c r="C761" t="s">
-        <v>2171</v>
       </c>
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
+        <v>2171</v>
+      </c>
+      <c r="B762" t="s">
         <v>2172</v>
       </c>
-      <c r="B762" t="s">
+      <c r="C762" t="s">
         <v>2173</v>
-      </c>
-      <c r="C762" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.25">
@@ -16834,29 +16816,29 @@
         <v>2190</v>
       </c>
       <c r="C768" t="s">
-        <v>2191</v>
+        <v>303</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
+        <v>2191</v>
+      </c>
+      <c r="B769" t="s">
         <v>2192</v>
       </c>
-      <c r="B769" t="s">
+      <c r="C769" t="s">
         <v>2193</v>
-      </c>
-      <c r="C769" t="s">
-        <v>2194</v>
       </c>
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
+        <v>2194</v>
+      </c>
+      <c r="B770" t="s">
         <v>2195</v>
       </c>
-      <c r="B770" t="s">
+      <c r="C770" t="s">
         <v>2196</v>
-      </c>
-      <c r="C770" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="771" spans="1:3" x14ac:dyDescent="0.25">
@@ -16867,29 +16849,29 @@
         <v>2198</v>
       </c>
       <c r="C771" t="s">
-        <v>2199</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
+        <v>2199</v>
+      </c>
+      <c r="B772" t="s">
         <v>2200</v>
       </c>
-      <c r="B772" t="s">
+      <c r="C772" t="s">
         <v>2201</v>
-      </c>
-      <c r="C772" t="s">
-        <v>2202</v>
       </c>
     </row>
     <row r="773" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B773" t="s">
         <v>2203</v>
       </c>
-      <c r="B773" t="s">
+      <c r="C773" t="s">
         <v>2204</v>
-      </c>
-      <c r="C773" t="s">
-        <v>1542</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.25">
@@ -16999,29 +16981,29 @@
         <v>2233</v>
       </c>
       <c r="C783" t="s">
-        <v>2234</v>
+        <v>509</v>
       </c>
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B784" t="s">
         <v>2235</v>
       </c>
-      <c r="B784" t="s">
+      <c r="C784" t="s">
         <v>2236</v>
-      </c>
-      <c r="C784" t="s">
-        <v>2237</v>
       </c>
     </row>
     <row r="785" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
+        <v>2237</v>
+      </c>
+      <c r="B785" t="s">
         <v>2238</v>
       </c>
-      <c r="B785" t="s">
+      <c r="C785" t="s">
         <v>2239</v>
-      </c>
-      <c r="C785" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.25">
@@ -17901,29 +17883,29 @@
         <v>2478</v>
       </c>
       <c r="C865" t="s">
-        <v>2479</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B866" t="s">
         <v>2480</v>
       </c>
-      <c r="B866" t="s">
+      <c r="C866" t="s">
         <v>2481</v>
-      </c>
-      <c r="C866" t="s">
-        <v>2482</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
+        <v>2482</v>
+      </c>
+      <c r="B867" t="s">
         <v>2483</v>
       </c>
-      <c r="B867" t="s">
+      <c r="C867" t="s">
         <v>2484</v>
-      </c>
-      <c r="C867" t="s">
-        <v>2467</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.25">
@@ -18496,28 +18478,6 @@
       </c>
       <c r="C919" t="s">
         <v>2640</v>
-      </c>
-    </row>
-    <row r="920" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A920" t="s">
-        <v>2641</v>
-      </c>
-      <c r="B920" t="s">
-        <v>2642</v>
-      </c>
-      <c r="C920" t="s">
-        <v>2643</v>
-      </c>
-    </row>
-    <row r="921" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A921" t="s">
-        <v>2644</v>
-      </c>
-      <c r="B921" t="s">
-        <v>2645</v>
-      </c>
-      <c r="C921" t="s">
-        <v>2646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove adobe acrobat sign
</commit_message>
<xml_diff>
--- a/add-in-ids/add-ins-using-exchange-tokens.xlsx
+++ b/add-in-ids/add-ins-using-exchange-tokens.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB031348-F088-4EA8-8002-58C2D4A3CF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C71497-A64B-4E37-AA78-608A70459B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="735" windowWidth="18615" windowHeight="14130" xr2:uid="{8FF931F1-CAD9-4954-9038-88E82260DB46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{8FF931F1-CAD9-4954-9038-88E82260DB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Add-ins list" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="2628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="2625">
   <si>
     <t>AssetID</t>
   </si>
@@ -1195,15 +1195,6 @@
   </si>
   <si>
     <t>simPRO</t>
-  </si>
-  <si>
-    <t>wa104381158</t>
-  </si>
-  <si>
-    <t>5DE11285-4132-4ADD-A025-EB72EB16BC84</t>
-  </si>
-  <si>
-    <t>Adobe Acrobat Sign</t>
   </si>
   <si>
     <t>wa104381160</t>
@@ -7999,8 +7990,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}" name="Table1" displayName="Table1" ref="A1:C914" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C914" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}" name="Table1" displayName="Table1" ref="A1:C913" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C913" xr:uid="{CD6B8178-56C6-442C-A6BF-7C2D1F869861}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{39B649A1-0CDF-46AA-A276-6F4F89255D96}" name="AssetID"/>
     <tableColumn id="2" xr3:uid="{C79A1EFF-47FF-488B-A562-E9848648C952}" name="AppId"/>
@@ -8327,10 +8318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3293B4AA-89CE-4E6A-9112-DA5B905DDA88}">
-  <dimension ref="A1:C914"/>
+  <dimension ref="A1:C913"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
-      <selection activeCell="A483" sqref="A483:XFD483"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:XFD132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8346,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2627</v>
+        <v>2624</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -10104,7 +10095,7 @@
       <c r="A162" t="s">
         <v>478</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="1" t="s">
         <v>479</v>
       </c>
       <c r="C162" t="s">
@@ -10115,7 +10106,7 @@
       <c r="A163" t="s">
         <v>481</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" t="s">
         <v>482</v>
       </c>
       <c r="C163" t="s">
@@ -10163,18 +10154,18 @@
         <v>494</v>
       </c>
       <c r="C167" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>495</v>
+      </c>
+      <c r="B168" t="s">
         <v>496</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>497</v>
-      </c>
-      <c r="C168" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -10809,18 +10800,18 @@
         <v>669</v>
       </c>
       <c r="B226" t="s">
+        <v>446</v>
+      </c>
+      <c r="C226" t="s">
         <v>670</v>
-      </c>
-      <c r="C226" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>671</v>
+      </c>
+      <c r="B227" t="s">
         <v>672</v>
-      </c>
-      <c r="B227" t="s">
-        <v>449</v>
       </c>
       <c r="C227" t="s">
         <v>673</v>
@@ -11414,15 +11405,15 @@
         <v>833</v>
       </c>
       <c r="B281" t="s">
-        <v>834</v>
+        <v>281</v>
       </c>
       <c r="C281" t="s">
-        <v>835</v>
+        <v>282</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B282" t="s">
         <v>281</v>
@@ -11433,7 +11424,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B283" t="s">
         <v>281</v>
@@ -11444,7 +11435,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B284" t="s">
         <v>281</v>
@@ -11455,7 +11446,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B285" t="s">
         <v>281</v>
@@ -11466,7 +11457,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B286" t="s">
         <v>281</v>
@@ -11477,13 +11468,13 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
+        <v>839</v>
+      </c>
+      <c r="B287" t="s">
+        <v>840</v>
+      </c>
+      <c r="C287" t="s">
         <v>841</v>
-      </c>
-      <c r="B287" t="s">
-        <v>281</v>
-      </c>
-      <c r="C287" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -11502,15 +11493,15 @@
         <v>845</v>
       </c>
       <c r="B289" t="s">
-        <v>846</v>
+        <v>281</v>
       </c>
       <c r="C289" t="s">
-        <v>847</v>
+        <v>282</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B290" t="s">
         <v>281</v>
@@ -11521,7 +11512,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B291" t="s">
         <v>281</v>
@@ -11532,7 +11523,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B292" t="s">
         <v>281</v>
@@ -11543,13 +11534,13 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
+        <v>849</v>
+      </c>
+      <c r="B293" t="s">
+        <v>850</v>
+      </c>
+      <c r="C293" t="s">
         <v>851</v>
-      </c>
-      <c r="B293" t="s">
-        <v>281</v>
-      </c>
-      <c r="C293" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -11568,21 +11559,21 @@
         <v>855</v>
       </c>
       <c r="B295" t="s">
-        <v>856</v>
+        <v>281</v>
       </c>
       <c r="C295" t="s">
-        <v>857</v>
+        <v>282</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
+        <v>856</v>
+      </c>
+      <c r="B296" t="s">
+        <v>857</v>
+      </c>
+      <c r="C296" t="s">
         <v>858</v>
-      </c>
-      <c r="B296" t="s">
-        <v>281</v>
-      </c>
-      <c r="C296" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -11590,15 +11581,15 @@
         <v>859</v>
       </c>
       <c r="B297" t="s">
-        <v>860</v>
+        <v>281</v>
       </c>
       <c r="C297" t="s">
-        <v>861</v>
+        <v>282</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B298" t="s">
         <v>281</v>
@@ -11609,13 +11600,13 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
+        <v>861</v>
+      </c>
+      <c r="B299" t="s">
+        <v>862</v>
+      </c>
+      <c r="C299" t="s">
         <v>863</v>
-      </c>
-      <c r="B299" t="s">
-        <v>281</v>
-      </c>
-      <c r="C299" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -11678,21 +11669,21 @@
         <v>879</v>
       </c>
       <c r="B305" t="s">
-        <v>880</v>
+        <v>281</v>
       </c>
       <c r="C305" t="s">
-        <v>881</v>
+        <v>282</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
+        <v>880</v>
+      </c>
+      <c r="B306" t="s">
+        <v>881</v>
+      </c>
+      <c r="C306" t="s">
         <v>882</v>
-      </c>
-      <c r="B306" t="s">
-        <v>281</v>
-      </c>
-      <c r="C306" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -11700,15 +11691,15 @@
         <v>883</v>
       </c>
       <c r="B307" t="s">
-        <v>884</v>
+        <v>281</v>
       </c>
       <c r="C307" t="s">
-        <v>885</v>
+        <v>282</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B308" t="s">
         <v>281</v>
@@ -11719,7 +11710,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B309" t="s">
         <v>281</v>
@@ -11730,7 +11721,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B310" t="s">
         <v>281</v>
@@ -11741,7 +11732,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B311" t="s">
         <v>281</v>
@@ -11752,7 +11743,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B312" t="s">
         <v>281</v>
@@ -11763,7 +11754,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B313" t="s">
         <v>281</v>
@@ -11774,7 +11765,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B314" t="s">
         <v>281</v>
@@ -11785,7 +11776,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B315" t="s">
         <v>281</v>
@@ -11796,7 +11787,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B316" t="s">
         <v>281</v>
@@ -11807,7 +11798,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B317" t="s">
         <v>281</v>
@@ -11818,7 +11809,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B318" t="s">
         <v>281</v>
@@ -11829,7 +11820,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="B319" t="s">
         <v>281</v>
@@ -11840,7 +11831,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B320" t="s">
         <v>281</v>
@@ -11851,7 +11842,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B321" t="s">
         <v>281</v>
@@ -11862,7 +11853,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B322" t="s">
         <v>281</v>
@@ -11873,7 +11864,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="B323" t="s">
         <v>281</v>
@@ -11884,7 +11875,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B324" t="s">
         <v>281</v>
@@ -11895,7 +11886,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B325" t="s">
         <v>281</v>
@@ -11906,7 +11897,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B326" t="s">
         <v>281</v>
@@ -11917,7 +11908,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B327" t="s">
         <v>281</v>
@@ -11928,7 +11919,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B328" t="s">
         <v>281</v>
@@ -11939,13 +11930,13 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
+        <v>905</v>
+      </c>
+      <c r="B329" t="s">
+        <v>906</v>
+      </c>
+      <c r="C329" t="s">
         <v>907</v>
-      </c>
-      <c r="B329" t="s">
-        <v>281</v>
-      </c>
-      <c r="C329" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -11953,15 +11944,15 @@
         <v>908</v>
       </c>
       <c r="B330" t="s">
-        <v>909</v>
+        <v>281</v>
       </c>
       <c r="C330" t="s">
-        <v>910</v>
+        <v>282</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B331" t="s">
         <v>281</v>
@@ -11972,7 +11963,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B332" t="s">
         <v>281</v>
@@ -11983,7 +11974,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B333" t="s">
         <v>281</v>
@@ -11994,7 +11985,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B334" t="s">
         <v>281</v>
@@ -12005,13 +11996,13 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
+        <v>913</v>
+      </c>
+      <c r="B335" t="s">
+        <v>914</v>
+      </c>
+      <c r="C335" t="s">
         <v>915</v>
-      </c>
-      <c r="B335" t="s">
-        <v>281</v>
-      </c>
-      <c r="C335" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -12019,15 +12010,15 @@
         <v>916</v>
       </c>
       <c r="B336" t="s">
-        <v>917</v>
+        <v>281</v>
       </c>
       <c r="C336" t="s">
-        <v>918</v>
+        <v>282</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B337" t="s">
         <v>281</v>
@@ -12038,13 +12029,13 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
+        <v>918</v>
+      </c>
+      <c r="B338" t="s">
+        <v>919</v>
+      </c>
+      <c r="C338" t="s">
         <v>920</v>
-      </c>
-      <c r="B338" t="s">
-        <v>281</v>
-      </c>
-      <c r="C338" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -12077,18 +12068,18 @@
         <v>928</v>
       </c>
       <c r="C341" t="s">
-        <v>929</v>
+        <v>282</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
+        <v>929</v>
+      </c>
+      <c r="B342" t="s">
         <v>930</v>
       </c>
-      <c r="B342" t="s">
+      <c r="C342" t="s">
         <v>931</v>
-      </c>
-      <c r="C342" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -12308,18 +12299,18 @@
         <v>990</v>
       </c>
       <c r="C362" t="s">
-        <v>991</v>
+        <v>282</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
+        <v>991</v>
+      </c>
+      <c r="B363" t="s">
         <v>992</v>
       </c>
-      <c r="B363" t="s">
+      <c r="C363" t="s">
         <v>993</v>
-      </c>
-      <c r="C363" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -12327,21 +12318,21 @@
         <v>994</v>
       </c>
       <c r="B364" t="s">
-        <v>995</v>
+        <v>38</v>
       </c>
       <c r="C364" t="s">
-        <v>996</v>
+        <v>39</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
+        <v>995</v>
+      </c>
+      <c r="B365" t="s">
+        <v>996</v>
+      </c>
+      <c r="C365" t="s">
         <v>997</v>
-      </c>
-      <c r="B365" t="s">
-        <v>38</v>
-      </c>
-      <c r="C365" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -12349,21 +12340,21 @@
         <v>998</v>
       </c>
       <c r="B366" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="C366" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
+        <v>999</v>
+      </c>
+      <c r="B367" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C367" t="s">
         <v>1001</v>
-      </c>
-      <c r="B367" t="s">
-        <v>999</v>
-      </c>
-      <c r="C367" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -12657,29 +12648,29 @@
         <v>1080</v>
       </c>
       <c r="B394" t="s">
-        <v>1081</v>
+        <v>990</v>
       </c>
       <c r="C394" t="s">
-        <v>1082</v>
+        <v>282</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="B395" t="s">
-        <v>993</v>
+        <v>203</v>
       </c>
       <c r="C395" t="s">
-        <v>282</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B396" t="s">
         <v>1084</v>
-      </c>
-      <c r="B396" t="s">
-        <v>203</v>
       </c>
       <c r="C396" t="s">
         <v>1085</v>
@@ -12899,18 +12890,18 @@
         <v>1143</v>
       </c>
       <c r="B416" t="s">
+        <v>634</v>
+      </c>
+      <c r="C416" t="s">
         <v>1144</v>
-      </c>
-      <c r="C416" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B417" t="s">
         <v>1146</v>
-      </c>
-      <c r="B417" t="s">
-        <v>637</v>
       </c>
       <c r="C417" t="s">
         <v>1147</v>
@@ -12997,7 +12988,7 @@
       <c r="A425" t="s">
         <v>1169</v>
       </c>
-      <c r="B425" t="s">
+      <c r="B425" s="1" t="s">
         <v>1170</v>
       </c>
       <c r="C425" t="s">
@@ -13008,7 +12999,7 @@
       <c r="A426" t="s">
         <v>1172</v>
       </c>
-      <c r="B426" s="1" t="s">
+      <c r="B426" t="s">
         <v>1173</v>
       </c>
       <c r="C426" t="s">
@@ -13129,7 +13120,7 @@
       <c r="A437" t="s">
         <v>1205</v>
       </c>
-      <c r="B437" t="s">
+      <c r="B437" s="1" t="s">
         <v>1206</v>
       </c>
       <c r="C437" t="s">
@@ -13140,7 +13131,7 @@
       <c r="A438" t="s">
         <v>1208</v>
       </c>
-      <c r="B438" s="1" t="s">
+      <c r="B438" t="s">
         <v>1209</v>
       </c>
       <c r="C438" t="s">
@@ -13217,7 +13208,7 @@
       <c r="A445" t="s">
         <v>1229</v>
       </c>
-      <c r="B445" t="s">
+      <c r="B445" s="1" t="s">
         <v>1230</v>
       </c>
       <c r="C445" t="s">
@@ -13228,7 +13219,7 @@
       <c r="A446" t="s">
         <v>1232</v>
       </c>
-      <c r="B446" s="1" t="s">
+      <c r="B446" t="s">
         <v>1233</v>
       </c>
       <c r="C446" t="s">
@@ -13437,7 +13428,7 @@
       <c r="A465" t="s">
         <v>1289</v>
       </c>
-      <c r="B465" t="s">
+      <c r="B465" s="1" t="s">
         <v>1290</v>
       </c>
       <c r="C465" t="s">
@@ -13448,7 +13439,7 @@
       <c r="A466" t="s">
         <v>1292</v>
       </c>
-      <c r="B466" s="1" t="s">
+      <c r="B466" t="s">
         <v>1293</v>
       </c>
       <c r="C466" t="s">
@@ -13580,7 +13571,7 @@
       <c r="A478" t="s">
         <v>1328</v>
       </c>
-      <c r="B478" t="s">
+      <c r="B478" s="1" t="s">
         <v>1329</v>
       </c>
       <c r="C478" t="s">
@@ -13591,7 +13582,7 @@
       <c r="A479" t="s">
         <v>1331</v>
       </c>
-      <c r="B479" s="1" t="s">
+      <c r="B479" t="s">
         <v>1332</v>
       </c>
       <c r="C479" t="s">
@@ -13622,13 +13613,13 @@
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="B482" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="C482" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.25">
@@ -13658,21 +13649,21 @@
         <v>1350</v>
       </c>
       <c r="B485" t="s">
-        <v>1351</v>
+        <v>990</v>
       </c>
       <c r="C485" t="s">
-        <v>1352</v>
+        <v>282</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B486" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C486" t="s">
         <v>1353</v>
-      </c>
-      <c r="B486" t="s">
-        <v>993</v>
-      </c>
-      <c r="C486" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
@@ -14255,18 +14246,18 @@
         <v>1511</v>
       </c>
       <c r="C539" t="s">
-        <v>1512</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B540" t="s">
         <v>1513</v>
       </c>
-      <c r="B540" t="s">
+      <c r="C540" t="s">
         <v>1514</v>
-      </c>
-      <c r="C540" t="s">
-        <v>1312</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.25">
@@ -14274,18 +14265,18 @@
         <v>1515</v>
       </c>
       <c r="B541" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C541" t="s">
         <v>1516</v>
-      </c>
-      <c r="C541" t="s">
-        <v>1517</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B542" t="s">
         <v>1518</v>
-      </c>
-      <c r="B542" t="s">
-        <v>1502</v>
       </c>
       <c r="C542" t="s">
         <v>1519</v>
@@ -14725,18 +14716,18 @@
         <v>1637</v>
       </c>
       <c r="B582" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C582" t="s">
         <v>1638</v>
-      </c>
-      <c r="C582" t="s">
-        <v>1639</v>
       </c>
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B583" t="s">
         <v>1640</v>
-      </c>
-      <c r="B583" t="s">
-        <v>1502</v>
       </c>
       <c r="C583" t="s">
         <v>1641</v>
@@ -15201,18 +15192,18 @@
         <v>1766</v>
       </c>
       <c r="C625" t="s">
-        <v>1767</v>
+        <v>614</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B626" t="s">
         <v>1768</v>
       </c>
-      <c r="B626" t="s">
+      <c r="C626" t="s">
         <v>1769</v>
-      </c>
-      <c r="C626" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.25">
@@ -15619,18 +15610,18 @@
         <v>1879</v>
       </c>
       <c r="C663" t="s">
-        <v>1880</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B664" t="s">
         <v>1881</v>
       </c>
-      <c r="B664" t="s">
+      <c r="C664" t="s">
         <v>1882</v>
-      </c>
-      <c r="C664" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.25">
@@ -15839,18 +15830,18 @@
         <v>1938</v>
       </c>
       <c r="C683" t="s">
-        <v>1939</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="684" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B684" t="s">
         <v>1940</v>
       </c>
-      <c r="B684" t="s">
+      <c r="C684" t="s">
         <v>1941</v>
-      </c>
-      <c r="C684" t="s">
-        <v>1395</v>
       </c>
     </row>
     <row r="685" spans="1:3" x14ac:dyDescent="0.25">
@@ -16631,18 +16622,18 @@
         <v>2153</v>
       </c>
       <c r="C755" t="s">
-        <v>2154</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
+        <v>2154</v>
+      </c>
+      <c r="B756" t="s">
         <v>2155</v>
       </c>
-      <c r="B756" t="s">
+      <c r="C756" t="s">
         <v>2156</v>
-      </c>
-      <c r="C756" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.25">
@@ -16719,18 +16710,18 @@
         <v>2176</v>
       </c>
       <c r="C763" t="s">
-        <v>2177</v>
+        <v>294</v>
       </c>
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
+        <v>2177</v>
+      </c>
+      <c r="B764" t="s">
         <v>2178</v>
       </c>
-      <c r="B764" t="s">
+      <c r="C764" t="s">
         <v>2179</v>
-      </c>
-      <c r="C764" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.25">
@@ -16752,18 +16743,18 @@
         <v>2184</v>
       </c>
       <c r="C766" t="s">
-        <v>2185</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
+        <v>2185</v>
+      </c>
+      <c r="B767" t="s">
         <v>2186</v>
       </c>
-      <c r="B767" t="s">
+      <c r="C767" t="s">
         <v>2187</v>
-      </c>
-      <c r="C767" t="s">
-        <v>1528</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.25">
@@ -16884,18 +16875,18 @@
         <v>2219</v>
       </c>
       <c r="C778" t="s">
-        <v>2220</v>
+        <v>497</v>
       </c>
     </row>
     <row r="779" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B779" t="s">
         <v>2221</v>
       </c>
-      <c r="B779" t="s">
+      <c r="C779" t="s">
         <v>2222</v>
-      </c>
-      <c r="C779" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="780" spans="1:3" x14ac:dyDescent="0.25">
@@ -17775,18 +17766,18 @@
         <v>2461</v>
       </c>
       <c r="C859" t="s">
-        <v>2462</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
+        <v>2462</v>
+      </c>
+      <c r="B860" t="s">
         <v>2463</v>
       </c>
-      <c r="B860" t="s">
+      <c r="C860" t="s">
         <v>2464</v>
-      </c>
-      <c r="C860" t="s">
-        <v>2447</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.25">
@@ -18370,17 +18361,6 @@
       </c>
       <c r="C913" t="s">
         <v>2623</v>
-      </c>
-    </row>
-    <row r="914" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A914" t="s">
-        <v>2624</v>
-      </c>
-      <c r="B914" t="s">
-        <v>2625</v>
-      </c>
-      <c r="C914" t="s">
-        <v>2626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>